<commit_message>
preparation release 101 0d30ff0387a24faed70d7649834eb335607b312a
</commit_message>
<xml_diff>
--- a/29-préparation-release-101/ig/StructureDefinition-tddui-bundle.xlsx
+++ b/29-préparation-release-101/ig/StructureDefinition-tddui-bundle.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>1.0.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-22T08:59:29+00:00</t>
+    <t>2025-09-22T09:16:12+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>